<commit_message>
industry exposure corrected, analysis 0 done and 1 progressed
</commit_message>
<xml_diff>
--- a/streamlit_review/anotations_dataset_metrics.xlsx
+++ b/streamlit_review/anotations_dataset_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguel/Documents/Master Thesis/Thesis/streamlit_review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129B28FB-6511-4640-A03C-F10ADA7E1715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12CADF0-AE5E-0E42-9A49-4012672EAA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="19940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulator" sheetId="1" r:id="rId1"/>
@@ -647,7 +647,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="20" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -732,7 +732,7 @@
       </c>
       <c r="E7" s="4">
         <f>SUMPRODUCT(E21:E23,$E$4:$E$6)</f>
-        <v>56010.703999999998</v>
+        <v>55815.856</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -836,11 +836,11 @@
         <v>94</v>
       </c>
       <c r="D22" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E22" s="8">
         <f>SUM(B22:D22)</f>
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F22" s="9">
         <f>$B$11</f>
@@ -848,7 +848,7 @@
       </c>
       <c r="G22" s="9">
         <f>E22-F22</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -862,11 +862,11 @@
         <v>4</v>
       </c>
       <c r="D23" s="6">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E23" s="8">
         <f>SUM(B23:D23)</f>
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F23" s="9">
         <f>$B$12</f>
@@ -874,7 +874,7 @@
       </c>
       <c r="G23" s="9">
         <f>E23-F23</f>
-        <v>-7</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -992,11 +992,11 @@
       </c>
       <c r="D30" s="4">
         <f>B22+D22</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" s="4">
         <f>$E$24-B30-C30-D30</f>
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F30" s="12">
         <f>IFERROR(B30/(B30+C30),"")</f>
@@ -1004,19 +1004,19 @@
       </c>
       <c r="G30" s="12">
         <f t="shared" si="0"/>
-        <v>0.8545454545454545</v>
+        <v>0.84684684684684686</v>
       </c>
       <c r="H30" s="12">
         <f t="shared" si="0"/>
-        <v>2.6470588235294117E-2</v>
+        <v>2.6548672566371681E-2</v>
       </c>
       <c r="I30" s="12">
         <f>IFERROR(E30/(E30+C30),"")</f>
-        <v>0.97352941176470587</v>
+        <v>0.97345132743362828</v>
       </c>
       <c r="J30" s="4">
         <f>E22</f>
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -1025,11 +1025,11 @@
       </c>
       <c r="B31" s="4">
         <f>D23</f>
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C31" s="4">
         <f>D21+D22</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D31" s="4">
         <f>B23+C23</f>
@@ -1041,23 +1041,23 @@
       </c>
       <c r="F31" s="12">
         <f>IFERROR(B31/(B31+C31),"")</f>
-        <v>0.94094488188976377</v>
+        <v>0.93700787401574803</v>
       </c>
       <c r="G31" s="12">
         <f t="shared" si="0"/>
-        <v>0.98353909465020573</v>
+        <v>0.98347107438016534</v>
       </c>
       <c r="H31" s="12">
         <f t="shared" si="0"/>
-        <v>7.2463768115942032E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="I31" s="12">
         <f>IFERROR(E31/(E31+C31),"")</f>
-        <v>0.92753623188405798</v>
+        <v>0.92307692307692313</v>
       </c>
       <c r="J31" s="4">
         <f>E23</f>
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="E33" s="14">
         <f>SUMPRODUCT(E21:E23,$E$4:$E$6)</f>
-        <v>56010.703999999998</v>
+        <v>55815.856</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="E36" s="4">
         <f>$E$33-B36-C36-D36</f>
-        <v>55533.383999999998</v>
+        <v>55338.536</v>
       </c>
       <c r="F36" s="12">
         <f>IFERROR(B36/(B36+C36),"")</f>
@@ -1136,11 +1136,11 @@
       </c>
       <c r="H36" s="12">
         <f t="shared" si="1"/>
-        <v>8.3915041130604769E-4</v>
+        <v>8.4210258716158992E-4</v>
       </c>
       <c r="I36" s="12">
         <f>IFERROR(E36/(E36+C36),"")</f>
-        <v>0.999160849588694</v>
+        <v>0.99915789741283845</v>
       </c>
       <c r="J36" s="4">
         <f>E21*$E$4</f>
@@ -1161,11 +1161,11 @@
       </c>
       <c r="D37" s="4">
         <f>(B22+D22)*$E$5</f>
-        <v>373.12</v>
+        <v>396.44</v>
       </c>
       <c r="E37" s="4">
         <f>$E$33-B37-C37-D37</f>
-        <v>52550.631999999991</v>
+        <v>52332.463999999993</v>
       </c>
       <c r="F37" s="12">
         <f>IFERROR(B37/(B37+C37),"")</f>
@@ -1173,19 +1173,19 @@
       </c>
       <c r="G37" s="12">
         <f t="shared" si="1"/>
-        <v>0.85454545454545461</v>
+        <v>0.84684684684684686</v>
       </c>
       <c r="H37" s="12">
         <f t="shared" si="1"/>
-        <v>1.6743634787315321E-2</v>
+        <v>1.681226353315898E-2</v>
       </c>
       <c r="I37" s="12">
         <f>IFERROR(E37/(E37+C37),"")</f>
-        <v>0.98325636521268467</v>
+        <v>0.98318773646684099</v>
       </c>
       <c r="J37" s="4">
         <f>E22*$E$5</f>
-        <v>2565.1999999999998</v>
+        <v>2588.52</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -1194,11 +1194,11 @@
       </c>
       <c r="B38" s="4">
         <f>D23*$E$6</f>
-        <v>52142.152000000002</v>
+        <v>51923.984000000004</v>
       </c>
       <c r="C38" s="4">
         <f>D21*$E$4 + D22*$E$5</f>
-        <v>330.92</v>
+        <v>354.24</v>
       </c>
       <c r="D38" s="4">
         <f>(B23+C23)*$E$6</f>
@@ -1210,23 +1210,23 @@
       </c>
       <c r="F38" s="12">
         <f>IFERROR(B38/(B38+C38),"")</f>
-        <v>0.9936935272247831</v>
+        <v>0.99322394731695551</v>
       </c>
       <c r="G38" s="12">
         <f t="shared" si="1"/>
-        <v>0.98353909465020584</v>
+        <v>0.98347107438016534</v>
       </c>
       <c r="H38" s="12">
         <f t="shared" si="1"/>
-        <v>0.11045836281827058</v>
+        <v>0.11732909379968219</v>
       </c>
       <c r="I38" s="12">
         <f>IFERROR(E38/(E38+C38),"")</f>
-        <v>0.88954163718172941</v>
+        <v>0.88267090620031774</v>
       </c>
       <c r="J38" s="4">
         <f>E23*$E$6</f>
-        <v>53014.824000000001</v>
+        <v>52796.656000000003</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="E44" s="4">
         <f>(C22+D22)*$E$5 + (C23+D23)*$E$6</f>
-        <v>55533.383999999998</v>
+        <v>55338.536</v>
       </c>
       <c r="F44" s="12">
         <f>IFERROR(B44/(B44+C44),"")</f>
@@ -1330,11 +1330,11 @@
       </c>
       <c r="H44" s="12">
         <f>IFERROR(C44/(C44+E44),"")</f>
-        <v>8.3915041130604769E-4</v>
+        <v>8.4210258716158992E-4</v>
       </c>
       <c r="I44" s="12">
         <f>IFERROR(E44/(E44+C44),"")</f>
-        <v>0.999160849588694</v>
+        <v>0.99915789741283845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>